<commit_message>
App created and most functionality added
</commit_message>
<xml_diff>
--- a/Example Schedule_Bookings.xlsx
+++ b/Example Schedule_Bookings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drjda\Movie-Schedule-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FC248A-8A10-4D70-B091-184AE27B02B0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CC9622-36BA-48E9-B64B-7FF58F16FF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{A789D899-18FF-4E4C-8F38-5B6A5489061F}"/>
+    <workbookView xWindow="-23385" yWindow="1440" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{A789D899-18FF-4E4C-8F38-5B6A5489061F}"/>
   </bookViews>
   <sheets>
     <sheet name="Film Details" sheetId="4" r:id="rId1"/>
@@ -22,10 +22,19 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Visualization Output'!$A$1:$AY$20</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -199,8 +208,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -313,18 +322,15 @@
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -339,9 +345,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -355,7 +358,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,14 +366,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4337,25 +4346,25 @@
   </sheetPr>
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E2" s="19" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -4368,204 +4377,204 @@
       <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="19"/>
+      <c r="E3" s="34"/>
       <c r="F3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="6.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="22">
         <v>1001</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>102</v>
       </c>
-      <c r="E5" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E5" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="22">
         <v>1002</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>91</v>
       </c>
-      <c r="E6" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E6" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="22">
         <v>1003</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>97</v>
       </c>
-      <c r="E7" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="22">
         <v>1004</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>120</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="22">
         <v>1005</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>128</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E9" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="22">
         <v>1006</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>113</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="22">
         <v>1007</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>104</v>
       </c>
-      <c r="E11" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="22">
         <v>1008</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>147</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="16"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="16"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="E12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4586,18 +4595,18 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
@@ -4605,7 +4614,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
@@ -4613,7 +4622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
@@ -4621,15 +4630,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4637,7 +4646,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4645,7 +4654,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -4653,7 +4662,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -4661,7 +4670,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -4669,7 +4678,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -4677,7 +4686,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -4685,7 +4694,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -4693,15 +4702,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -4709,7 +4718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -4717,7 +4726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -4741,468 +4750,468 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.90625" customWidth="1"/>
-    <col min="10" max="10" width="7.1796875" customWidth="1"/>
-    <col min="11" max="11" width="1.36328125" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" customWidth="1"/>
-    <col min="13" max="13" width="9.81640625" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
+    <col min="11" max="11" width="1.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>0.54166666666666663</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>0.94791666666666663</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="L8" s="10" t="s">
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="L8" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:14" s="13" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="M8" s="35"/>
+    </row>
+    <row r="9" spans="1:14" s="12" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="12" t="s">
+      <c r="K9" s="17"/>
+      <c r="L9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <v>4</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="14">
-        <v>30</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="E10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="13">
+        <v>30</v>
+      </c>
+      <c r="H10" s="13">
         <v>20</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <v>102</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="14">
         <v>15</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K10" s="13"/>
+      <c r="L10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>4</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="14">
-        <v>30</v>
-      </c>
-      <c r="H11" s="14">
+      <c r="E11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="13">
+        <v>30</v>
+      </c>
+      <c r="H11" s="13">
         <v>20</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="13">
         <v>91</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="14">
         <v>15</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N11" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K11" s="13"/>
+      <c r="L11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>4</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="14">
-        <v>30</v>
-      </c>
-      <c r="H12" s="14">
+      <c r="E12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="13">
+        <v>30</v>
+      </c>
+      <c r="H12" s="13">
         <v>20</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="13">
         <v>97</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="14">
         <v>15</v>
       </c>
-      <c r="K12" s="14"/>
-      <c r="L12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K12" s="13"/>
+      <c r="L12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="14">
         <v>4</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="14">
-        <v>30</v>
-      </c>
-      <c r="H13" s="14">
+      <c r="E13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="13">
+        <v>30</v>
+      </c>
+      <c r="H13" s="13">
         <v>20</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="13">
         <v>120</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="14">
         <v>15</v>
       </c>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K13" s="13"/>
+      <c r="L13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="14">
         <v>4</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="14">
-        <v>30</v>
-      </c>
-      <c r="H14" s="14">
+      <c r="E14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="13">
+        <v>30</v>
+      </c>
+      <c r="H14" s="13">
         <v>20</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <v>128</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="14">
         <v>15</v>
       </c>
-      <c r="L14" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <v>4</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="14">
-        <v>30</v>
-      </c>
-      <c r="H15" s="14">
+      <c r="E15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="13">
+        <v>30</v>
+      </c>
+      <c r="H15" s="13">
         <v>20</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="13">
         <v>113</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="14">
         <v>15</v>
       </c>
-      <c r="L15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="14">
         <v>4</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="14">
-        <v>30</v>
-      </c>
-      <c r="H16" s="14">
+      <c r="E16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="13">
+        <v>30</v>
+      </c>
+      <c r="H16" s="13">
         <v>20</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <v>104</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="14">
         <v>15</v>
       </c>
-      <c r="L16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N16" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>4</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="14">
-        <v>30</v>
-      </c>
-      <c r="H17" s="14">
+      <c r="E17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="13">
+        <v>30</v>
+      </c>
+      <c r="H17" s="13">
         <v>20</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="13">
         <v>147</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="14">
         <v>15</v>
       </c>
-      <c r="L17" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="M17" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="N17" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C18" s="14"/>
+      <c r="L17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5227,26 +5236,26 @@
       <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5260,7 +5269,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5274,7 +5283,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -5288,7 +5297,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -5302,7 +5311,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -5317,7 +5326,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -5331,7 +5340,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -5345,7 +5354,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -5359,7 +5368,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -5374,7 +5383,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -5388,7 +5397,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -5402,7 +5411,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -5416,7 +5425,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -5430,7 +5439,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -5445,7 +5454,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -5459,7 +5468,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -5473,7 +5482,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -5487,7 +5496,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -5501,7 +5510,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -5515,7 +5524,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -5529,7 +5538,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -5543,7 +5552,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -5557,7 +5566,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -5571,7 +5580,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -5585,7 +5594,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -5599,7 +5608,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -5613,7 +5622,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -5627,7 +5636,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -5641,7 +5650,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -5655,7 +5664,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -5669,7 +5678,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -5683,7 +5692,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -5697,7 +5706,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -5724,482 +5733,482 @@
   </sheetPr>
   <dimension ref="A1:AW34"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="40" width="3.7265625" bestFit="1" customWidth="1"/>
-    <col min="41" max="49" width="3.54296875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="1.81640625" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="40" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="49" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="1.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="32">
+      <c r="B1" s="30">
         <v>1215</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="30">
         <v>1230</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="30">
         <v>1245</v>
       </c>
-      <c r="E1" s="33">
+      <c r="E1" s="31">
         <v>100</v>
       </c>
-      <c r="F1" s="34">
+      <c r="F1" s="32">
         <f>E1+15</f>
         <v>115</v>
       </c>
-      <c r="G1" s="34">
+      <c r="G1" s="32">
         <f t="shared" ref="G1:AV1" si="0">F1+15</f>
         <v>130</v>
       </c>
-      <c r="H1" s="34">
+      <c r="H1" s="32">
         <f t="shared" si="0"/>
         <v>145</v>
       </c>
-      <c r="I1" s="34">
+      <c r="I1" s="32">
         <v>200</v>
       </c>
-      <c r="J1" s="34">
+      <c r="J1" s="32">
         <f t="shared" si="0"/>
         <v>215</v>
       </c>
-      <c r="K1" s="34">
+      <c r="K1" s="32">
         <f t="shared" si="0"/>
         <v>230</v>
       </c>
-      <c r="L1" s="34">
+      <c r="L1" s="32">
         <f t="shared" si="0"/>
         <v>245</v>
       </c>
-      <c r="M1" s="34">
+      <c r="M1" s="32">
         <v>300</v>
       </c>
-      <c r="N1" s="34">
+      <c r="N1" s="32">
         <f t="shared" si="0"/>
         <v>315</v>
       </c>
-      <c r="O1" s="34">
+      <c r="O1" s="32">
         <f t="shared" si="0"/>
         <v>330</v>
       </c>
-      <c r="P1" s="34">
+      <c r="P1" s="32">
         <f t="shared" si="0"/>
         <v>345</v>
       </c>
-      <c r="Q1" s="34">
+      <c r="Q1" s="32">
         <v>400</v>
       </c>
-      <c r="R1" s="34">
+      <c r="R1" s="32">
         <f t="shared" si="0"/>
         <v>415</v>
       </c>
-      <c r="S1" s="34">
+      <c r="S1" s="32">
         <f t="shared" si="0"/>
         <v>430</v>
       </c>
-      <c r="T1" s="34">
+      <c r="T1" s="32">
         <f t="shared" si="0"/>
         <v>445</v>
       </c>
-      <c r="U1" s="34">
+      <c r="U1" s="32">
         <v>500</v>
       </c>
-      <c r="V1" s="34">
+      <c r="V1" s="32">
         <f t="shared" si="0"/>
         <v>515</v>
       </c>
-      <c r="W1" s="34">
+      <c r="W1" s="32">
         <f t="shared" si="0"/>
         <v>530</v>
       </c>
-      <c r="X1" s="34">
+      <c r="X1" s="32">
         <f t="shared" si="0"/>
         <v>545</v>
       </c>
-      <c r="Y1" s="34">
+      <c r="Y1" s="32">
         <v>600</v>
       </c>
-      <c r="Z1" s="34">
+      <c r="Z1" s="32">
         <f t="shared" si="0"/>
         <v>615</v>
       </c>
-      <c r="AA1" s="34">
+      <c r="AA1" s="32">
         <f t="shared" si="0"/>
         <v>630</v>
       </c>
-      <c r="AB1" s="34">
+      <c r="AB1" s="32">
         <f t="shared" si="0"/>
         <v>645</v>
       </c>
-      <c r="AC1" s="34">
+      <c r="AC1" s="32">
         <v>700</v>
       </c>
-      <c r="AD1" s="34">
+      <c r="AD1" s="32">
         <f t="shared" si="0"/>
         <v>715</v>
       </c>
-      <c r="AE1" s="34">
+      <c r="AE1" s="32">
         <f t="shared" si="0"/>
         <v>730</v>
       </c>
-      <c r="AF1" s="34">
+      <c r="AF1" s="32">
         <f t="shared" si="0"/>
         <v>745</v>
       </c>
-      <c r="AG1" s="34">
+      <c r="AG1" s="32">
         <v>800</v>
       </c>
-      <c r="AH1" s="34">
+      <c r="AH1" s="32">
         <f t="shared" si="0"/>
         <v>815</v>
       </c>
-      <c r="AI1" s="34">
+      <c r="AI1" s="32">
         <f t="shared" si="0"/>
         <v>830</v>
       </c>
-      <c r="AJ1" s="34">
+      <c r="AJ1" s="32">
         <f t="shared" si="0"/>
         <v>845</v>
       </c>
-      <c r="AK1" s="34">
+      <c r="AK1" s="32">
         <v>900</v>
       </c>
-      <c r="AL1" s="34">
+      <c r="AL1" s="32">
         <f t="shared" si="0"/>
         <v>915</v>
       </c>
-      <c r="AM1" s="34">
+      <c r="AM1" s="32">
         <f t="shared" si="0"/>
         <v>930</v>
       </c>
-      <c r="AN1" s="34">
+      <c r="AN1" s="32">
         <f t="shared" si="0"/>
         <v>945</v>
       </c>
-      <c r="AO1" s="35">
+      <c r="AO1" s="33">
         <v>1000</v>
       </c>
-      <c r="AP1" s="35">
+      <c r="AP1" s="33">
         <f t="shared" si="0"/>
         <v>1015</v>
       </c>
-      <c r="AQ1" s="35">
+      <c r="AQ1" s="33">
         <f t="shared" si="0"/>
         <v>1030</v>
       </c>
-      <c r="AR1" s="35">
+      <c r="AR1" s="33">
         <f t="shared" si="0"/>
         <v>1045</v>
       </c>
-      <c r="AS1" s="35">
+      <c r="AS1" s="33">
         <v>1100</v>
       </c>
-      <c r="AT1" s="35">
+      <c r="AT1" s="33">
         <f t="shared" si="0"/>
         <v>1115</v>
       </c>
-      <c r="AU1" s="35">
+      <c r="AU1" s="33">
         <f t="shared" si="0"/>
         <v>1130</v>
       </c>
-      <c r="AV1" s="35">
+      <c r="AV1" s="33">
         <f t="shared" si="0"/>
         <v>1145</v>
       </c>
-      <c r="AW1" s="35">
+      <c r="AW1" s="33">
         <v>1200</v>
       </c>
     </row>
-    <row r="2" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28">
+    <row r="2" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-    </row>
-    <row r="3" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+    </row>
+    <row r="3" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-    </row>
-    <row r="4" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="28">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-    </row>
-    <row r="6" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-    </row>
-    <row r="7" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="28">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="28">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-    </row>
-    <row r="9" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="28">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+    </row>
+    <row r="9" spans="1:49" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-    </row>
-    <row r="11" spans="1:49" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+    </row>
+    <row r="11" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="30">
         <v>1215</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="30">
         <v>1230</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="30">
         <v>1245</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="31">
         <v>100</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="32">
         <f>E11+15</f>
         <v>115</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="32">
         <f t="shared" ref="G11:AV11" si="1">F11+15</f>
         <v>130</v>
       </c>
-      <c r="H11" s="34">
+      <c r="H11" s="32">
         <f t="shared" si="1"/>
         <v>145</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="32">
         <v>200</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="32">
         <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="K11" s="34">
+      <c r="K11" s="32">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="32">
         <f t="shared" si="1"/>
         <v>245</v>
       </c>
-      <c r="M11" s="34">
+      <c r="M11" s="32">
         <v>300</v>
       </c>
-      <c r="N11" s="34">
+      <c r="N11" s="32">
         <f t="shared" si="1"/>
         <v>315</v>
       </c>
-      <c r="O11" s="34">
+      <c r="O11" s="32">
         <f t="shared" si="1"/>
         <v>330</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="32">
         <f t="shared" si="1"/>
         <v>345</v>
       </c>
-      <c r="Q11" s="34">
+      <c r="Q11" s="32">
         <v>400</v>
       </c>
-      <c r="R11" s="34">
+      <c r="R11" s="32">
         <f t="shared" si="1"/>
         <v>415</v>
       </c>
-      <c r="S11" s="34">
+      <c r="S11" s="32">
         <f t="shared" si="1"/>
         <v>430</v>
       </c>
-      <c r="T11" s="34">
+      <c r="T11" s="32">
         <f t="shared" si="1"/>
         <v>445</v>
       </c>
-      <c r="U11" s="34">
+      <c r="U11" s="32">
         <v>500</v>
       </c>
-      <c r="V11" s="34">
+      <c r="V11" s="32">
         <f t="shared" si="1"/>
         <v>515</v>
       </c>
-      <c r="W11" s="34">
+      <c r="W11" s="32">
         <f t="shared" si="1"/>
         <v>530</v>
       </c>
-      <c r="X11" s="34">
+      <c r="X11" s="32">
         <f t="shared" si="1"/>
         <v>545</v>
       </c>
-      <c r="Y11" s="34">
+      <c r="Y11" s="32">
         <v>600</v>
       </c>
-      <c r="Z11" s="34">
+      <c r="Z11" s="32">
         <f t="shared" si="1"/>
         <v>615</v>
       </c>
-      <c r="AA11" s="34">
+      <c r="AA11" s="32">
         <f t="shared" si="1"/>
         <v>630</v>
       </c>
-      <c r="AB11" s="34">
+      <c r="AB11" s="32">
         <f t="shared" si="1"/>
         <v>645</v>
       </c>
-      <c r="AC11" s="34">
+      <c r="AC11" s="32">
         <v>700</v>
       </c>
-      <c r="AD11" s="34">
+      <c r="AD11" s="32">
         <f t="shared" si="1"/>
         <v>715</v>
       </c>
-      <c r="AE11" s="34">
+      <c r="AE11" s="32">
         <f t="shared" si="1"/>
         <v>730</v>
       </c>
-      <c r="AF11" s="34">
+      <c r="AF11" s="32">
         <f t="shared" si="1"/>
         <v>745</v>
       </c>
-      <c r="AG11" s="34">
+      <c r="AG11" s="32">
         <v>800</v>
       </c>
-      <c r="AH11" s="34">
+      <c r="AH11" s="32">
         <f t="shared" si="1"/>
         <v>815</v>
       </c>
-      <c r="AI11" s="34">
+      <c r="AI11" s="32">
         <f t="shared" si="1"/>
         <v>830</v>
       </c>
-      <c r="AJ11" s="34">
+      <c r="AJ11" s="32">
         <f t="shared" si="1"/>
         <v>845</v>
       </c>
-      <c r="AK11" s="34">
+      <c r="AK11" s="32">
         <v>900</v>
       </c>
-      <c r="AL11" s="34">
+      <c r="AL11" s="32">
         <f t="shared" si="1"/>
         <v>915</v>
       </c>
-      <c r="AM11" s="34">
+      <c r="AM11" s="32">
         <f t="shared" si="1"/>
         <v>930</v>
       </c>
-      <c r="AN11" s="34">
+      <c r="AN11" s="32">
         <f t="shared" si="1"/>
         <v>945</v>
       </c>
-      <c r="AO11" s="35">
+      <c r="AO11" s="33">
         <v>1000</v>
       </c>
-      <c r="AP11" s="35">
+      <c r="AP11" s="33">
         <f t="shared" si="1"/>
         <v>1015</v>
       </c>
-      <c r="AQ11" s="35">
+      <c r="AQ11" s="33">
         <f t="shared" si="1"/>
         <v>1030</v>
       </c>
-      <c r="AR11" s="35">
+      <c r="AR11" s="33">
         <f t="shared" si="1"/>
         <v>1045</v>
       </c>
-      <c r="AS11" s="35">
+      <c r="AS11" s="33">
         <v>1100</v>
       </c>
-      <c r="AT11" s="35">
+      <c r="AT11" s="33">
         <f t="shared" si="1"/>
         <v>1115</v>
       </c>
-      <c r="AU11" s="35">
+      <c r="AU11" s="33">
         <f t="shared" si="1"/>
         <v>1130</v>
       </c>
-      <c r="AV11" s="35">
+      <c r="AV11" s="33">
         <f t="shared" si="1"/>
         <v>1145</v>
       </c>
-      <c r="AW11" s="35">
+      <c r="AW11" s="33">
         <v>1200</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A12" s="28">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
         <v>1</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
       <c r="G12" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
       <c r="S12" t="s">
         <v>51</v>
       </c>
@@ -6210,23 +6219,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A13" s="28">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
         <v>2</v>
       </c>
       <c r="F13" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30" t="s">
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="R13" s="30"/>
+      <c r="R13" s="28"/>
       <c r="AD13" t="s">
         <v>51</v>
       </c>
@@ -6234,21 +6243,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A14" s="28">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
         <v>3</v>
       </c>
       <c r="H14" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
       <c r="T14" t="s">
         <v>51</v>
       </c>
@@ -6259,21 +6268,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A15" s="28">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
         <v>4</v>
       </c>
       <c r="F15" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
       <c r="U15" t="s">
         <v>51</v>
       </c>
@@ -6284,21 +6293,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A16" s="28">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
         <v>5</v>
       </c>
       <c r="I16" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
       <c r="S16" t="s">
         <v>51</v>
       </c>
@@ -6309,21 +6318,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A17" s="28">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
         <v>6</v>
       </c>
       <c r="H17" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
       <c r="T17" t="s">
         <v>51</v>
       </c>
@@ -6334,23 +6343,23 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A18" s="28">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
         <v>7</v>
       </c>
       <c r="E18" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30" t="s">
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="R18" s="30"/>
+      <c r="R18" s="28"/>
       <c r="AB18" t="s">
         <v>51</v>
       </c>
@@ -6358,68 +6367,68 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="A19" s="28">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
         <v>8</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="31"/>
-      <c r="R19" s="31" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
-      <c r="AA19" s="13"/>
-      <c r="AB19" s="13"/>
-      <c r="AC19" s="13"/>
-      <c r="AD19" s="13"/>
-      <c r="AE19" s="13" t="s">
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="12"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12"/>
+      <c r="AD19" s="12"/>
+      <c r="AE19" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AF19" s="13"/>
-      <c r="AG19" s="13"/>
-      <c r="AH19" s="13"/>
-      <c r="AI19" s="13"/>
-      <c r="AJ19" s="13"/>
-      <c r="AK19" s="13"/>
-      <c r="AL19" s="13"/>
-      <c r="AM19" s="13"/>
-      <c r="AN19" s="13"/>
-      <c r="AO19" s="13"/>
-      <c r="AP19" s="13"/>
-      <c r="AQ19" s="13" t="s">
+      <c r="AF19" s="12"/>
+      <c r="AG19" s="12"/>
+      <c r="AH19" s="12"/>
+      <c r="AI19" s="12"/>
+      <c r="AJ19" s="12"/>
+      <c r="AK19" s="12"/>
+      <c r="AL19" s="12"/>
+      <c r="AM19" s="12"/>
+      <c r="AN19" s="12"/>
+      <c r="AO19" s="12"/>
+      <c r="AP19" s="12"/>
+      <c r="AQ19" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AR19" s="13"/>
-      <c r="AS19" s="13"/>
-      <c r="AT19" s="13"/>
-      <c r="AU19" s="13"/>
-      <c r="AV19" s="13"/>
-      <c r="AW19" s="13"/>
-    </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.35">
+      <c r="AR19" s="12"/>
+      <c r="AS19" s="12"/>
+      <c r="AT19" s="12"/>
+      <c r="AU19" s="12"/>
+      <c r="AV19" s="12"/>
+      <c r="AW19" s="12"/>
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -6438,16 +6447,16 @@
       <c r="I20">
         <v>1</v>
       </c>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30">
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28">
         <v>2</v>
       </c>
-      <c r="R20" s="30">
+      <c r="R20" s="28">
         <v>1</v>
       </c>
       <c r="S20">
@@ -6490,139 +6499,139 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-    </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-    </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-    </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-    </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="30"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
-    </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-    </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-    </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30"/>
-      <c r="P28" s="30"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-    </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30"/>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
-    </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-    </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="29"/>
-    </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.35">
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
-    </row>
-    <row r="33" spans="11:18" x14ac:dyDescent="0.35">
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-    </row>
-    <row r="34" spans="11:18" x14ac:dyDescent="0.35">
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+    </row>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+    </row>
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="28"/>
+    </row>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+    </row>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="28"/>
+    </row>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
+    </row>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
+    </row>
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
+    </row>
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+    </row>
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+    </row>
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+    </row>
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+    </row>
+    <row r="33" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+    </row>
+    <row r="34" spans="11:18" x14ac:dyDescent="0.25">
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>